<commit_message>
coordinating the scripts with the repos
</commit_message>
<xml_diff>
--- a/subjects.xlsx
+++ b/subjects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\B-D_EEG_Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>name</t>
   </si>
@@ -45,69 +45,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1002</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1003</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1004</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1005</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1007</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1008</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1010</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1012</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1013</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1015</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1016</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1018</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1020</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1021</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1022</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1023</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1025</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1027</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1029</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1030</t>
-  </si>
-  <si>
-    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\EEG_Data\1017</t>
-  </si>
-  <si>
     <t>sub</t>
   </si>
   <si>
@@ -172,6 +109,135 @@
   </si>
   <si>
     <t>sub-21</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-01</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-02</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-03</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-04</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-05</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-06</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-07</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-08</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-09</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-10</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-11</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-12</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-13</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-14</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-15</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-16</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-17</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-18</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-19</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-20</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-21</t>
+  </si>
+  <si>
+    <t>raw_data</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-01</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-02</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-03</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-04</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-05</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-06</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-07</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-08</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-09</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-10</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-11</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-12</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-13</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-14</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-15</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-16</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-17</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-18</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-19</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-20</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-21</t>
   </si>
 </sst>
 </file>
@@ -979,15 +1045,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1007,15 +1073,18 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1002</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1030,15 +1099,18 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1003</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1053,15 +1125,18 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1004</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1076,15 +1151,18 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1005</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1099,15 +1177,18 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1007</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1122,15 +1203,18 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1008</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1145,15 +1229,18 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1010</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1168,15 +1255,18 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1012</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1191,15 +1281,18 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1013</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1214,15 +1307,18 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1015</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1237,15 +1333,18 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1016</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1260,15 +1359,18 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1017</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1283,15 +1385,18 @@
         <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1018</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1306,15 +1411,18 @@
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1020</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1329,15 +1437,18 @@
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1021</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1352,15 +1463,18 @@
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1022</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1375,15 +1489,18 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1023</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1398,15 +1515,18 @@
         <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="H18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1025</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1421,15 +1541,18 @@
         <v>6</v>
       </c>
       <c r="G19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1027</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1444,15 +1567,18 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1029</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1467,15 +1593,18 @@
         <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="H21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1030</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1490,7 +1619,10 @@
         <v>6</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the baseline recording analyses to the repo
</commit_message>
<xml_diff>
--- a/subjects.xlsx
+++ b/subjects.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="95">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>folder</t>
-  </si>
-  <si>
     <t>group</t>
   </si>
   <si>
@@ -238,6 +235,75 @@
   </si>
   <si>
     <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\BIDS_data\bids\sourcedata\sub-21</t>
+  </si>
+  <si>
+    <t>folder_int</t>
+  </si>
+  <si>
+    <t>folder_baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-01\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-02\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-03\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-04\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-05\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-06\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-07\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-08\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-09\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-10\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-11\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-12\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-13\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-14\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-15\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-16\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-17\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-18\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-19\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-20\Baseline</t>
+  </si>
+  <si>
+    <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-21\Baseline</t>
   </si>
 </sst>
 </file>
@@ -1045,584 +1111,650 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1002</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1003</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1004</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4">
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1005</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>7</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1007</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1008</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1010</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1012</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1013</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1015</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>7</v>
       </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1016</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12">
+      <c r="F12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>7</v>
       </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1017</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>6</v>
       </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1018</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14">
+      <c r="F14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14">
         <v>0</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>6</v>
       </c>
-      <c r="G14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1020</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>5</v>
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>8</v>
       </c>
-      <c r="G15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1021</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>8</v>
       </c>
-      <c r="G16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1022</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
         <v>7</v>
       </c>
-      <c r="G17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1023</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18">
         <v>2</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18">
+      <c r="F18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18">
         <v>0</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>6</v>
       </c>
-      <c r="G18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1025</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19">
+      <c r="F19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19">
         <v>0</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>6</v>
       </c>
-      <c r="G19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1027</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20">
         <v>2</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
+      <c r="F20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
         <v>7</v>
       </c>
-      <c r="G20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1029</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
+      <c r="F21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
         <v>7</v>
       </c>
-      <c r="G21" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1030</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>5</v>
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
       </c>
       <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22">
         <v>0</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <v>6</v>
       </c>
-      <c r="G22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" t="s">
-        <v>72</v>
+      <c r="I22" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(hopefully) final coordination of files and scripts for sharing
</commit_message>
<xml_diff>
--- a/subjects.xlsx
+++ b/subjects.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
   <si>
     <t>name</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>I:\SCIENCE-NEXS-neurolab\PROJECTS\PLAYMORE\EEG_project1\Analyses\OSF_files\EEG_derivatives\sub-21\Baseline</t>
+  </si>
+  <si>
+    <t>included</t>
   </si>
 </sst>
 </file>
@@ -1111,15 +1114,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,8 +1150,11 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1002</v>
       </c>
@@ -1176,8 +1182,11 @@
       <c r="I2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1003</v>
       </c>
@@ -1205,8 +1214,11 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1004</v>
       </c>
@@ -1234,8 +1246,11 @@
       <c r="I4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1005</v>
       </c>
@@ -1263,8 +1278,11 @@
       <c r="I5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1007</v>
       </c>
@@ -1292,8 +1310,11 @@
       <c r="I6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1008</v>
       </c>
@@ -1321,8 +1342,11 @@
       <c r="I7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1010</v>
       </c>
@@ -1350,8 +1374,11 @@
       <c r="I8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1012</v>
       </c>
@@ -1379,8 +1406,11 @@
       <c r="I9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1013</v>
       </c>
@@ -1408,8 +1438,11 @@
       <c r="I10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1015</v>
       </c>
@@ -1437,8 +1470,11 @@
       <c r="I11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1016</v>
       </c>
@@ -1466,8 +1502,11 @@
       <c r="I12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1017</v>
       </c>
@@ -1495,8 +1534,11 @@
       <c r="I13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1018</v>
       </c>
@@ -1524,8 +1566,11 @@
       <c r="I14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1020</v>
       </c>
@@ -1553,8 +1598,11 @@
       <c r="I15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1021</v>
       </c>
@@ -1582,8 +1630,11 @@
       <c r="I16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1022</v>
       </c>
@@ -1611,8 +1662,11 @@
       <c r="I17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1023</v>
       </c>
@@ -1640,8 +1694,11 @@
       <c r="I18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1025</v>
       </c>
@@ -1669,8 +1726,11 @@
       <c r="I19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1027</v>
       </c>
@@ -1698,8 +1758,11 @@
       <c r="I20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1029</v>
       </c>
@@ -1727,8 +1790,11 @@
       <c r="I21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1030</v>
       </c>
@@ -1755,6 +1821,9 @@
       </c>
       <c r="I22" t="s">
         <v>28</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>